<commit_message>
added moves and backup database
</commit_message>
<xml_diff>
--- a/res/Docs/PokemonBST(Master).xlsx
+++ b/res/Docs/PokemonBST(Master).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cole\Documents\Unity\Roguelike\res\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E842779-B319-4747-A915-109570596BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB88C12-E381-44DA-BA20-46AE1ED4CA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{95CD4222-BC88-4298-AA5E-3BACFDC62B97}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{95CD4222-BC88-4298-AA5E-3BACFDC62B97}"/>
   </bookViews>
   <sheets>
     <sheet name="Pokemon" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="202">
   <si>
     <t>Pokemon name</t>
   </si>
@@ -604,6 +604,45 @@
   </si>
   <si>
     <t>normal psychic</t>
+  </si>
+  <si>
+    <t>Ice</t>
+  </si>
+  <si>
+    <t>Aurora Beam</t>
+  </si>
+  <si>
+    <t>Blizzard</t>
+  </si>
+  <si>
+    <t>Hail</t>
+  </si>
+  <si>
+    <t>Ice Ball</t>
+  </si>
+  <si>
+    <t>Haze</t>
+  </si>
+  <si>
+    <t>Ice Beam</t>
+  </si>
+  <si>
+    <t>Ice Punch</t>
+  </si>
+  <si>
+    <t>Icicle Spear</t>
+  </si>
+  <si>
+    <t>Icy Wind</t>
+  </si>
+  <si>
+    <t>Mist</t>
+  </si>
+  <si>
+    <t>Powder Snow</t>
+  </si>
+  <si>
+    <t>Sheer Cold</t>
   </si>
 </sst>
 </file>
@@ -977,7 +1016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4CBEF43-B3F9-4B93-9787-764E8C86EDE9}">
   <dimension ref="A1:M124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+    <sheetView topLeftCell="A70" workbookViewId="0">
       <selection activeCell="G96" sqref="G96"/>
     </sheetView>
   </sheetViews>
@@ -4983,10 +5022,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF3FAE6-6540-4B9B-A3F6-6B3804427797}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="U28" sqref="U28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5618,6 +5657,246 @@
         <v>158</v>
       </c>
     </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>190</v>
+      </c>
+      <c r="B32" t="s">
+        <v>189</v>
+      </c>
+      <c r="C32">
+        <v>20</v>
+      </c>
+      <c r="D32">
+        <v>65</v>
+      </c>
+      <c r="E32">
+        <v>100</v>
+      </c>
+      <c r="F32" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>191</v>
+      </c>
+      <c r="B33" t="s">
+        <v>189</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>120</v>
+      </c>
+      <c r="E33">
+        <v>70</v>
+      </c>
+      <c r="F33" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34" t="s">
+        <v>189</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>100</v>
+      </c>
+      <c r="F34" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>194</v>
+      </c>
+      <c r="B35" t="s">
+        <v>189</v>
+      </c>
+      <c r="C35">
+        <v>30</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>100</v>
+      </c>
+      <c r="F35" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>193</v>
+      </c>
+      <c r="B36" t="s">
+        <v>189</v>
+      </c>
+      <c r="C36">
+        <v>20</v>
+      </c>
+      <c r="D36">
+        <v>30</v>
+      </c>
+      <c r="E36">
+        <v>90</v>
+      </c>
+      <c r="F36" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>195</v>
+      </c>
+      <c r="B37" t="s">
+        <v>189</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+      <c r="D37">
+        <v>95</v>
+      </c>
+      <c r="E37">
+        <v>100</v>
+      </c>
+      <c r="F37" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>196</v>
+      </c>
+      <c r="B38" t="s">
+        <v>189</v>
+      </c>
+      <c r="C38">
+        <v>15</v>
+      </c>
+      <c r="D38">
+        <v>75</v>
+      </c>
+      <c r="E38">
+        <v>100</v>
+      </c>
+      <c r="F38" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>197</v>
+      </c>
+      <c r="B39" t="s">
+        <v>189</v>
+      </c>
+      <c r="C39">
+        <v>30</v>
+      </c>
+      <c r="D39">
+        <v>10</v>
+      </c>
+      <c r="E39">
+        <v>100</v>
+      </c>
+      <c r="F39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>198</v>
+      </c>
+      <c r="B40" t="s">
+        <v>189</v>
+      </c>
+      <c r="C40">
+        <v>15</v>
+      </c>
+      <c r="D40">
+        <v>55</v>
+      </c>
+      <c r="E40">
+        <v>95</v>
+      </c>
+      <c r="F40" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>199</v>
+      </c>
+      <c r="B41" t="s">
+        <v>189</v>
+      </c>
+      <c r="C41">
+        <v>30</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>100</v>
+      </c>
+      <c r="F41" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>200</v>
+      </c>
+      <c r="B42" t="s">
+        <v>189</v>
+      </c>
+      <c r="C42">
+        <v>25</v>
+      </c>
+      <c r="D42">
+        <v>40</v>
+      </c>
+      <c r="E42">
+        <v>100</v>
+      </c>
+      <c r="F42" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>201</v>
+      </c>
+      <c r="B43" t="s">
+        <v>189</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>138</v>
+      </c>
+      <c r="E43">
+        <v>30</v>
+      </c>
+      <c r="F43" t="s">
+        <v>159</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added MoveCatagory and made moves physical, special or other
</commit_message>
<xml_diff>
--- a/res/Docs/PokemonBST(Master).xlsx
+++ b/res/Docs/PokemonBST(Master).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cole\Documents\Unity\Roguelike\res\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB88C12-E381-44DA-BA20-46AE1ED4CA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0537704E-6692-4204-B505-7B07F69C0633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{95CD4222-BC88-4298-AA5E-3BACFDC62B97}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{95CD4222-BC88-4298-AA5E-3BACFDC62B97}"/>
   </bookViews>
   <sheets>
     <sheet name="Pokemon" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="213">
   <si>
     <t>Pokemon name</t>
   </si>
@@ -643,6 +643,39 @@
   </si>
   <si>
     <t>Sheer Cold</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>Fury Cutter</t>
+  </si>
+  <si>
+    <t>Leech Life</t>
+  </si>
+  <si>
+    <t>Megahorn</t>
+  </si>
+  <si>
+    <t>Pin Missile</t>
+  </si>
+  <si>
+    <t>Signal Beam</t>
+  </si>
+  <si>
+    <t>Silver Wind</t>
+  </si>
+  <si>
+    <t>Spider Web</t>
+  </si>
+  <si>
+    <t>String Shot</t>
+  </si>
+  <si>
+    <t>Tail Glow</t>
+  </si>
+  <si>
+    <t>Twineedle</t>
   </si>
 </sst>
 </file>
@@ -1016,8 +1049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4CBEF43-B3F9-4B93-9787-764E8C86EDE9}">
   <dimension ref="A1:M124"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="G96" sqref="G96"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,6 +2286,9 @@
       <c r="J36" t="s">
         <v>188</v>
       </c>
+      <c r="K36" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -2285,6 +2321,9 @@
       </c>
       <c r="J37" t="s">
         <v>188</v>
+      </c>
+      <c r="K37" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -4979,9 +5018,6 @@
       <c r="I118">
         <f t="shared" si="5"/>
         <v>0</v>
-      </c>
-      <c r="K118" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
@@ -5022,16 +5058,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF3FAE6-6540-4B9B-A3F6-6B3804427797}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="U28" sqref="U28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5887,14 +5924,214 @@
       <c r="C43">
         <v>5</v>
       </c>
-      <c r="D43" t="s">
-        <v>138</v>
+      <c r="D43">
+        <v>0</v>
       </c>
       <c r="E43">
         <v>30</v>
       </c>
       <c r="F43" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>203</v>
+      </c>
+      <c r="B44" t="s">
+        <v>202</v>
+      </c>
+      <c r="C44">
+        <v>20</v>
+      </c>
+      <c r="D44">
+        <v>10</v>
+      </c>
+      <c r="E44">
+        <v>95</v>
+      </c>
+      <c r="F44" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>204</v>
+      </c>
+      <c r="B45" t="s">
+        <v>202</v>
+      </c>
+      <c r="C45">
+        <v>15</v>
+      </c>
+      <c r="D45">
+        <v>20</v>
+      </c>
+      <c r="E45">
+        <v>100</v>
+      </c>
+      <c r="F45" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>205</v>
+      </c>
+      <c r="B46" t="s">
+        <v>202</v>
+      </c>
+      <c r="C46">
+        <v>10</v>
+      </c>
+      <c r="D46">
+        <v>120</v>
+      </c>
+      <c r="E46">
+        <v>85</v>
+      </c>
+      <c r="F46" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>206</v>
+      </c>
+      <c r="B47" t="s">
+        <v>202</v>
+      </c>
+      <c r="C47">
+        <v>20</v>
+      </c>
+      <c r="D47">
+        <v>14</v>
+      </c>
+      <c r="E47">
+        <v>85</v>
+      </c>
+      <c r="F47" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>207</v>
+      </c>
+      <c r="B48" t="s">
+        <v>202</v>
+      </c>
+      <c r="C48">
+        <v>15</v>
+      </c>
+      <c r="D48">
+        <v>75</v>
+      </c>
+      <c r="E48">
+        <v>100</v>
+      </c>
+      <c r="F48" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>208</v>
+      </c>
+      <c r="B49" t="s">
+        <v>202</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+      <c r="D49">
+        <v>60</v>
+      </c>
+      <c r="E49">
+        <v>100</v>
+      </c>
+      <c r="F49" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>209</v>
+      </c>
+      <c r="B50" t="s">
+        <v>202</v>
+      </c>
+      <c r="C50">
+        <v>10</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>100</v>
+      </c>
+      <c r="F50" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>210</v>
+      </c>
+      <c r="B51" t="s">
+        <v>202</v>
+      </c>
+      <c r="C51">
+        <v>40</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>95</v>
+      </c>
+      <c r="F51" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>211</v>
+      </c>
+      <c r="B52" t="s">
+        <v>202</v>
+      </c>
+      <c r="C52">
+        <v>20</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>100</v>
+      </c>
+      <c r="F52" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>212</v>
+      </c>
+      <c r="B53" t="s">
+        <v>202</v>
+      </c>
+      <c r="C53">
+        <v>20</v>
+      </c>
+      <c r="D53">
+        <v>25</v>
+      </c>
+      <c r="E53">
+        <v>100</v>
+      </c>
+      <c r="F53" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented party selection hud
</commit_message>
<xml_diff>
--- a/res/Docs/PokemonBST(Master).xlsx
+++ b/res/Docs/PokemonBST(Master).xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cole\Documents\Unity\Roguelike\res\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0537704E-6692-4204-B505-7B07F69C0633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A61BD89-15DE-4DE4-BBAB-EED11B8527C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{95CD4222-BC88-4298-AA5E-3BACFDC62B97}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{95CD4222-BC88-4298-AA5E-3BACFDC62B97}"/>
   </bookViews>
   <sheets>
     <sheet name="Pokemon" sheetId="1" r:id="rId1"/>
     <sheet name="Moves" sheetId="2" r:id="rId2"/>
+    <sheet name="Stages" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="271">
   <si>
     <t>Pokemon name</t>
   </si>
@@ -676,6 +677,180 @@
   </si>
   <si>
     <t>Twineedle</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Item Pool</t>
+  </si>
+  <si>
+    <t>NPC Pool</t>
+  </si>
+  <si>
+    <t>Overworld Objects</t>
+  </si>
+  <si>
+    <t>Special Event</t>
+  </si>
+  <si>
+    <t>Pallet Town</t>
+  </si>
+  <si>
+    <t>Your house, Rival's house, Lab</t>
+  </si>
+  <si>
+    <t>Choose starter</t>
+  </si>
+  <si>
+    <t>Map:20, Potion:100, Pokeballs(5):100, Pokedex:100</t>
+  </si>
+  <si>
+    <t>Oak, Rival, Mom, Rival's Sister</t>
+  </si>
+  <si>
+    <t>Veridian City</t>
+  </si>
+  <si>
+    <t>Gym, Pokemart, Pokecenter</t>
+  </si>
+  <si>
+    <t>Catch Tutorial(50/50 MasterBall or dud ball):50</t>
+  </si>
+  <si>
+    <t>potion:40 dreameater/will-o-wisp50/50: 100 (behind surf/cut)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Giovanni, Old man, </t>
+  </si>
+  <si>
+    <t>Veridian Forrest</t>
+  </si>
+  <si>
+    <t>Wild Pokemons</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Bug Catchers</t>
+  </si>
+  <si>
+    <t>Caterpie:20, Weedle:20, Pikachu:3, Metapod:15, Kakuna:15, Pidgey:20, Pidgeotto:7</t>
+  </si>
+  <si>
+    <t>antidote:100, pokeballs(5):20, Bug Buzz: 10, cheri berries(4):20, Tiny Mushroom: 20</t>
+  </si>
+  <si>
+    <t>Pewder City</t>
+  </si>
+  <si>
+    <t>Museum, Pokecenter, Pokemart, Gym</t>
+  </si>
+  <si>
+    <t>Fossil(Old Amber):10</t>
+  </si>
+  <si>
+    <t>Brock, Oak Aid</t>
+  </si>
+  <si>
+    <t>Mt. Moon</t>
+  </si>
+  <si>
+    <t>Join/Fight Rocket:25</t>
+  </si>
+  <si>
+    <t>Lass:20, Scientist:40, Hiker:40</t>
+  </si>
+  <si>
+    <t>Onix:15, Clefairy:5, Paris:10, Zubat:40, Geodude:30</t>
+  </si>
+  <si>
+    <t>Fossil(helix/Dome):100, Rare Candy:40, Bullet Seed:30, Water Gun:20 Revive:25, HP UP:10, Pokeball(5):30</t>
+  </si>
+  <si>
+    <t>Cerulean City</t>
+  </si>
+  <si>
+    <t>Rival, Rocket Grunt</t>
+  </si>
+  <si>
+    <t>Nugget Bridge/Route 24</t>
+  </si>
+  <si>
+    <t>Oddish:35, Abra:10, Bellsprout:35, Venonat:20</t>
+  </si>
+  <si>
+    <t>Nugget:100, SS Anne ticket</t>
+  </si>
+  <si>
+    <t>BILL's House</t>
+  </si>
+  <si>
+    <t>Vermillian City</t>
+  </si>
+  <si>
+    <t>Squirtle(egg move):33</t>
+  </si>
+  <si>
+    <t>Bulbasaur(egg move):33</t>
+  </si>
+  <si>
+    <t>Join/Fight Rocket:25, Charmander(egg move):33</t>
+  </si>
+  <si>
+    <t>Bike Voucher:100</t>
+  </si>
+  <si>
+    <t>Bike Shop, Gym, Pokecenter, Pokemart</t>
+  </si>
+  <si>
+    <t>Diglett:80, Dugtrio:20</t>
+  </si>
+  <si>
+    <t>Diglett Cave (caved in)</t>
+  </si>
+  <si>
+    <t>Power Plant</t>
+  </si>
+  <si>
+    <t>ThunderBolt:40, Thundershock:70, Paralyze Heal:100, pokeball(5):100, if Item is rolled -&gt; Electrode:30</t>
+  </si>
+  <si>
+    <t>Voltorb:20, Pikachu:50, Electabuzz:30</t>
+  </si>
+  <si>
+    <t>Rock Tunnel</t>
+  </si>
+  <si>
+    <t>Hiker, Fire Breather</t>
+  </si>
+  <si>
+    <t>EvoStone: 40, Vitamin:40, Rock Slide:30, Metal Coat:20</t>
+  </si>
+  <si>
+    <t>Machop:15, Gravelor:25, Onix:35, Zubat:20, Magmar:5</t>
+  </si>
+  <si>
+    <t>Lavender Town</t>
+  </si>
+  <si>
+    <t>Lavender Tower</t>
+  </si>
+  <si>
+    <t>Lavender Tower, Pokemart, Pokecenter</t>
+  </si>
+  <si>
+    <t>Mediums</t>
+  </si>
+  <si>
+    <t>Gastly:60, Cubone:25, Haunter:15</t>
+  </si>
+  <si>
+    <t>Marowak(silphScope)</t>
+  </si>
+  <si>
+    <t>PokeFlute:100, Shadow Tag:40</t>
   </si>
 </sst>
 </file>
@@ -5060,7 +5235,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF3FAE6-6540-4B9B-A3F6-6B3804427797}">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -6137,4 +6312,301 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38B12F8A-DDED-42DB-97C0-6F8632DA67B4}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="94.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" customWidth="1"/>
+    <col min="5" max="5" width="76.7109375" customWidth="1"/>
+    <col min="6" max="6" width="44" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D2" t="s">
+        <v>219</v>
+      </c>
+      <c r="E2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E3" t="s">
+        <v>230</v>
+      </c>
+      <c r="F3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D4" t="s">
+        <v>230</v>
+      </c>
+      <c r="E4" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D5" t="s">
+        <v>235</v>
+      </c>
+      <c r="E5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" t="s">
+        <v>242</v>
+      </c>
+      <c r="C6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D6" t="s">
+        <v>230</v>
+      </c>
+      <c r="E6" t="s">
+        <v>241</v>
+      </c>
+      <c r="F6" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D7" t="s">
+        <v>254</v>
+      </c>
+      <c r="E7" t="s">
+        <v>230</v>
+      </c>
+      <c r="F7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>245</v>
+      </c>
+      <c r="B8" t="s">
+        <v>247</v>
+      </c>
+      <c r="C8" t="s">
+        <v>244</v>
+      </c>
+      <c r="D8" t="s">
+        <v>248</v>
+      </c>
+      <c r="E8" t="s">
+        <v>246</v>
+      </c>
+      <c r="F8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>249</v>
+      </c>
+      <c r="B9" t="s">
+        <v>253</v>
+      </c>
+      <c r="C9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D9" t="s">
+        <v>224</v>
+      </c>
+      <c r="E9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>256</v>
+      </c>
+      <c r="B10" t="s">
+        <v>230</v>
+      </c>
+      <c r="C10" t="s">
+        <v>230</v>
+      </c>
+      <c r="D10" t="s">
+        <v>230</v>
+      </c>
+      <c r="E10" t="s">
+        <v>255</v>
+      </c>
+      <c r="F10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>257</v>
+      </c>
+      <c r="B11" t="s">
+        <v>258</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>230</v>
+      </c>
+      <c r="E11" t="s">
+        <v>259</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>260</v>
+      </c>
+      <c r="B12" t="s">
+        <v>262</v>
+      </c>
+      <c r="C12" t="s">
+        <v>261</v>
+      </c>
+      <c r="D12" t="s">
+        <v>230</v>
+      </c>
+      <c r="E12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F12" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>264</v>
+      </c>
+      <c r="B13" t="s">
+        <v>230</v>
+      </c>
+      <c r="C13" t="s">
+        <v>230</v>
+      </c>
+      <c r="D13" t="s">
+        <v>266</v>
+      </c>
+      <c r="E13" t="s">
+        <v>230</v>
+      </c>
+      <c r="F13" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>265</v>
+      </c>
+      <c r="B14" t="s">
+        <v>270</v>
+      </c>
+      <c r="C14" t="s">
+        <v>267</v>
+      </c>
+      <c r="D14" t="s">
+        <v>230</v>
+      </c>
+      <c r="E14" t="s">
+        <v>268</v>
+      </c>
+      <c r="F14" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>